<commit_message>
Fixes a bug in chem constraint and also new constraints added.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -522,26 +522,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kalvin Phillips</t>
+          <t>Stefan Ortega</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -560,11 +560,11 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -583,38 +583,38 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="P2" t="n">
         <v>700</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>262</v>
+        <v>514</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Victor Lindelöf</t>
+          <t>Karim Adeyemi</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
         <v>3</v>
       </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
       <c r="F3" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -623,56 +623,56 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Non Rare</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
           <t>Med</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
       <c r="P3" t="n">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>309</v>
+        <v>812</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sven Botman</t>
+          <t>Niklas Stark</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -696,30 +696,30 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Newcastle Utd</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Non Rare</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -729,108 +729,108 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="P4" t="n">
         <v>650</v>
       </c>
       <c r="Q4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>333</v>
+        <v>2016</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Renan Lodi</t>
+          <t>Marc-Oliver Kempf</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
+        <v>75</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>gold</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Hertha Berlin</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>27</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Rare</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Med</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>650</v>
+      </c>
+      <c r="Q5" t="n">
         <v>3</v>
-      </c>
-      <c r="F5" t="n">
-        <v>80</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Premier League</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Nott'm Forest</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Brazil</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>24</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Rare</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Left</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
-      <c r="P5" t="n">
-        <v>750</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2721</v>
+        <v>2101</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sergi Roberto</t>
+          <t>Ridle Baku</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>RB</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>80</v>
@@ -842,25 +842,25 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FC Barcelona</t>
+          <t>VfL Wolfsburg</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Non Rare</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -870,7 +870,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -882,54 +882,54 @@
         <v>700</v>
       </c>
       <c r="Q6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4045</v>
+        <v>2599</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kangin Lee</t>
+          <t>David Neres</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>RW</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
         <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>silver</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Liga NOS (POR 1)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>RCD Mallorca</t>
+          <t>SL Benfica</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -948,7 +948,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="P7" t="n">
@@ -960,23 +960,23 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4318</v>
+        <v>2601</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Óscar Trejo</t>
+          <t>Lucas Veríssimo</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>79</v>
@@ -988,21 +988,21 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Liga NOS (POR 1)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Rayo Vallecano</t>
+          <t>SL Benfica</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -1021,38 +1021,38 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>High</t>
         </is>
       </c>
       <c r="P8" t="n">
         <v>700</v>
       </c>
       <c r="Q8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4355</v>
+        <v>3003</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Youssef En-Nesyri</t>
+          <t>Petr Ševčík</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1061,30 +1061,30 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Česká Liga (CZE 1)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Sevilla FC</t>
+          <t>Slavia Praha</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Czech Republic</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Non Rare</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1098,7 +1098,7 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="Q9" t="n">
         <v>2</v>
@@ -1106,26 +1106,26 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7552</v>
+        <v>3007</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mauro Arambarri</t>
+          <t>Lukas Provod</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1134,44 +1134,44 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Česká Liga (CZE 1)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Getafe CF</t>
+          <t>Slavia Praha</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Czech Republic</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Non Rare</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>High</t>
         </is>
       </c>
       <c r="P10" t="n">
-        <v>550</v>
+        <v>650</v>
       </c>
       <c r="Q10" t="n">
         <v>2</v>
@@ -1179,26 +1179,26 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7578</v>
+        <v>4780</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lucas Robertone</t>
+          <t>Salem Al Dawsari</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>LW</t>
         </is>
       </c>
       <c r="D11" t="n">
         <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1207,21 +1207,21 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>MBS Pro League (SAU 1)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>UD Almería</t>
+          <t>Al Hilal</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1247,80 +1247,80 @@
         <v>700</v>
       </c>
       <c r="Q11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8820</v>
+        <v>9424</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ledesma</t>
+          <t>Ruben Vargas</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>LM</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>75</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>gold</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FC Augsburg</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Switzerland</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>24</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Rare</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Med</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>650</v>
+      </c>
+      <c r="Q12" t="n">
         <v>2</v>
-      </c>
-      <c r="F12" t="n">
-        <v>80</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>LaLiga Santander</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Cádiz CF</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Argentina</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>29</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Non Rare</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Right</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
-      <c r="P12" t="n">
-        <v>500</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Experimental] Now players don't need to be fixed to their positions.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,29 +519,34 @@
           <t>Chemistry</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Is_Pos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>514</v>
+        <v>486</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Karim Adeyemi</t>
+          <t>Jamal Musiala</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,7 +560,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>FC Bayern</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -564,7 +569,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -573,12 +578,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -587,92 +592,98 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="Q2" t="n">
         <v>3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>562</v>
+        <v>514</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mark Flekken</t>
+          <t>Karim Adeyemi</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>75</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>gold</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Dortmund</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>21</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Rare</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Med</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>650</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3</v>
+      </c>
+      <c r="R3" t="n">
         <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" t="n">
-        <v>80</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Bundesliga</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>SC Freiburg</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>29</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Rare</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Right</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
-      <c r="P3" t="n">
-        <v>700</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>812</v>
+        <v>542</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Niklas Stark</t>
+          <t>Ko Itakura</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -681,10 +692,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>75</v>
@@ -701,16 +712,16 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>M'gladbach</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -737,30 +748,33 @@
       </c>
       <c r="Q4" t="n">
         <v>3</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2016</v>
+        <v>562</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Marc-Oliver Kempf</t>
+          <t>Mark Flekken</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -774,16 +788,16 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Hertha Berlin</t>
+          <t>SC Freiburg</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -792,12 +806,12 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -806,34 +820,37 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="Q5" t="n">
         <v>3</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2046</v>
+        <v>812</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anton Stach</t>
+          <t>Niklas Stark</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -847,7 +864,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1. FSV Mainz 05</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -856,7 +873,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -870,43 +887,46 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="Q6" t="n">
         <v>3</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2101</v>
+        <v>2016</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ridle Baku</t>
+          <t>Marc-Oliver Kempf</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -920,7 +940,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>VfL Wolfsburg</t>
+          <t>Hertha Berlin</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -929,7 +949,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -938,7 +958,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -952,34 +972,37 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="Q7" t="n">
         <v>3</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3521</v>
+        <v>2101</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bruma</t>
+          <t>Ridle Baku</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>LW</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
         <v>4</v>
       </c>
-      <c r="E8" t="n">
-        <v>3</v>
-      </c>
       <c r="F8" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -988,21 +1011,21 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Süper Lig (TUR 1)</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Fenerbahçe</t>
+          <t>VfL Wolfsburg</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -1021,35 +1044,38 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="P8" t="n">
         <v>700</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6491</v>
+        <v>2372</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jean-Daniel Akpa Akpro</t>
+          <t>Josip Šutalo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>75</v>
@@ -1061,21 +1087,21 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Serie A TIM</t>
+          <t>Liga Hrvatska (CRO 1)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Empoli</t>
+          <t>Dinamo Zagreb</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Côte d'Ivoire</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1089,7 +1115,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1101,31 +1127,34 @@
         <v>650</v>
       </c>
       <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7709</v>
+        <v>8198</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sebastián Palacios</t>
+          <t>Rico Henry</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RW</t>
+          <t>LWB</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1134,21 +1163,21 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Hellas Liga (GRE 1)</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Panathinaikos</t>
+          <t>Brentford</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>England</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1157,7 +1186,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1167,38 +1196,41 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>High</t>
         </is>
       </c>
       <c r="P10" t="n">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9044</v>
+        <v>8821</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Kevin Akpoguma</t>
+          <t>Alfonso Espino</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="D11" t="n">
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1207,21 +1239,21 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>LaLiga Santander</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>TSG Hoffenheim</t>
+          <t>Cádiz CF</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1230,24 +1262,27 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Left</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
           <t>Med</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>Med</t>
-        </is>
-      </c>
       <c r="P11" t="n">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="Q11" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1321,6 +1356,9 @@
       </c>
       <c r="Q12" t="n">
         <v>3</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a better way to model squad_rating constraint. Thanks `jacobi from EasySBC`.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -833,7 +833,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aidoo</t>
+          <t>Pereyra</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -851,22 +851,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Serie A TIM</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>RC Celta</t>
+          <t>Udinese</t>
         </is>
       </c>
       <c r="I8" t="n">

</xml_diff>

<commit_message>
Add early stopping and some comments.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -503,11 +503,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gosens</t>
+          <t>Pope</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -521,26 +521,26 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>LWB</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>England</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Serie A TIM</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Inter</t>
+          <t>Newcastle Utd</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>950</v>
+        <v>900</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -549,20 +549,20 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tah</t>
+          <t>Savanier</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -576,26 +576,26 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CAM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Montpellier</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -604,16 +604,16 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tapsoba</t>
+          <t>Akanji</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -636,21 +636,21 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Burkina Faso</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -668,7 +668,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Musiala</t>
+          <t>Upamecano</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -686,12 +686,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -714,20 +714,20 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Benítez</t>
+          <t>Keïta</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -741,26 +741,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Guinea</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Eredivisie</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>PSV</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" t="n">
         <v>1</v>
@@ -778,7 +778,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Aguerd</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -796,26 +796,26 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>VfL Wolfsburg</t>
+          <t>West Ham</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -833,7 +833,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Golovin</t>
+          <t>Fofana</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -851,26 +851,26 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>AS Monaco</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>1</v>
@@ -888,7 +888,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ito</t>
+          <t>Almirón</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -906,22 +906,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RW</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Stade de Reims</t>
+          <t>Newcastle Utd</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
         <v>1</v>
@@ -943,7 +943,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Teze</t>
+          <t>Oxlade-Chamberlain</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -961,26 +961,26 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>England</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Eredivisie</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>PSV</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M10" t="n">
         <v>1</v>
@@ -998,11 +998,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Stach</t>
+          <t>Rosier</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1016,26 +1016,26 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Süper Lig</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1. FSV Mainz 05</t>
+          <t>Beşiktaş</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -1044,20 +1044,20 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Boadu</t>
+          <t>Edouard</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1076,21 +1076,21 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>AS Monaco</t>
+          <t>Crystal Palace</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Significant speedup of `squad_rating_constraint`🚄
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Prioritize Duplicates and other changes.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,25 +476,35 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Untradeable</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Loans</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IsDuplicate</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IsInActive11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Cost</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>IsUntradable</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>IsLoaned</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Chemistry</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Is_Pos</t>
         </is>
@@ -503,11 +513,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Iñigo Martínez</t>
+          <t>Tapsoba</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -516,7 +526,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -526,43 +536,49 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Burkina Faso</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Athletic Club</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1100</v>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" t="n">
-        <v>3</v>
+      <c r="L2" t="b">
+        <v>0</v>
       </c>
       <c r="M2" t="n">
+        <v>750</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>David Soria</t>
+          <t>Upamecano</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -571,53 +587,59 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Getafe CF</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>1100</v>
+          <t>FC Bayern München</t>
+        </is>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N3" t="n">
         <v>3</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Gabriel Paulista</t>
+          <t>Lafont</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -626,53 +648,59 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Valencia CF</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>950</v>
+          <t>FC Nantes</t>
+        </is>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
         <v>0</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>700</v>
+      </c>
+      <c r="N4" t="n">
         <v>3</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ismaily</t>
+          <t>Guendouzi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -681,17 +709,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -701,29 +729,35 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>LOSC Lille</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>750</v>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="b">
         <v>0</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" t="b">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>800</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Matheus Reis</t>
+          <t>Bellarabi</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -736,49 +770,55 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Liga Portugal</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Sporting CP</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>750</v>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" t="b">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>700</v>
+      </c>
+      <c r="N6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Marcão</t>
+          <t>Gouiri</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -791,49 +831,55 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Sevilla FC</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>800</v>
+          <t>Stade Rennais FC</t>
+        </is>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="b">
         <v>0</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>700</v>
+      </c>
+      <c r="N7" t="n">
         <v>3</v>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>David Neres</t>
+          <t>Fofana</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -846,53 +892,59 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>RW</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Liga Portugal</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>SL Benfica</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>750</v>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
       </c>
-      <c r="L8" t="n">
-        <v>1</v>
+      <c r="L8" t="b">
+        <v>0</v>
       </c>
       <c r="M8" t="n">
+        <v>700</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Portu</t>
+          <t>Golovin</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -901,49 +953,55 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>LM</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>LaLiga Santander</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Getafe CF</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>800</v>
+          <t>AS Monaco</t>
+        </is>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="b">
         <v>0</v>
       </c>
-      <c r="L9" t="n">
-        <v>3</v>
+      <c r="L9" t="b">
+        <v>0</v>
       </c>
       <c r="M9" t="n">
+        <v>700</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Watkins</t>
+          <t>Ito</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -956,49 +1014,55 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>RW</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>750</v>
+          <t>Stade de Reims</t>
+        </is>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="b">
         <v>0</v>
       </c>
-      <c r="L10" t="n">
-        <v>3</v>
+      <c r="L10" t="b">
+        <v>0</v>
       </c>
       <c r="M10" t="n">
+        <v>700</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2</v>
+      </c>
+      <c r="O10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Oxlade-Chamberlain</t>
+          <t>Rosier</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1011,53 +1075,59 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Süper Lig</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>1100</v>
+          <t>Beşiktaş</t>
+        </is>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
       </c>
       <c r="J11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="b">
         <v>0</v>
       </c>
-      <c r="L11" t="n">
-        <v>2</v>
+      <c r="L11" t="b">
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>700</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ramsey</t>
+          <t>Stach</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1066,7 +1136,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>RARE</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1076,32 +1146,38 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>800</v>
+          <t>1. FSV Mainz 05</t>
+        </is>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
       </c>
-      <c r="L12" t="n">
-        <v>3</v>
+      <c r="L12" t="b">
+        <v>0</v>
       </c>
       <c r="M12" t="n">
+        <v>700</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
`EA FC 24` changes 📈
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -461,63 +461,63 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Is_Pos</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Country</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>League</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Club</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Untradeable</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Loans</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>IsDuplicate</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>IsInActive11</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Cost</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Is_Pos</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tapsoba</t>
+          <t>Shaw</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -534,26 +534,26 @@
           <t>CB</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Burkina Faso</t>
-        </is>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
-        </is>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Manchester Utd</t>
+        </is>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -561,24 +561,24 @@
       <c r="L2" t="b">
         <v>0</v>
       </c>
-      <c r="M2" t="n">
-        <v>750</v>
+      <c r="M2" t="b">
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>2</v>
+        <v>900</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Upamecano</t>
+          <t>Gerard Moreno</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -592,29 +592,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CB</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
+          <t>ST</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>FC Bayern München</t>
-        </is>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
+          <t>LALIGA EA SPORTS</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Villarreal CF</t>
+        </is>
       </c>
       <c r="J3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -622,24 +622,24 @@
       <c r="L3" t="b">
         <v>0</v>
       </c>
-      <c r="M3" t="n">
-        <v>1000</v>
+      <c r="M3" t="b">
+        <v>0</v>
       </c>
       <c r="N3" t="n">
+        <v>900</v>
+      </c>
+      <c r="O3" t="n">
         <v>3</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lafont</t>
+          <t>González</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -648,34 +648,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>GK</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
+          <t>LW</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>FC Nantes</t>
-        </is>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
+          <t>Serie A TIM</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="b">
         <v>0</v>
@@ -683,20 +683,20 @@
       <c r="L4" t="b">
         <v>0</v>
       </c>
-      <c r="M4" t="n">
-        <v>700</v>
+      <c r="M4" t="b">
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Guendouzi</t>
+          <t>Savanier</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -714,29 +714,29 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CM</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+          <t>CAM</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>France</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>OM</t>
-        </is>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="b">
         <v>0</v>
@@ -744,20 +744,20 @@
       <c r="L5" t="b">
         <v>0</v>
       </c>
-      <c r="M5" t="n">
-        <v>800</v>
+      <c r="M5" t="b">
+        <v>0</v>
       </c>
       <c r="N5" t="n">
+        <v>700</v>
+      </c>
+      <c r="O5" t="n">
         <v>3</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bellarabi</t>
+          <t>Mandanda</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -770,34 +770,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RM</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
+          <t>GK</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
-        </is>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
+          <t>Ligue 1 Uber Eats</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Stade Rennais FC</t>
+        </is>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -805,20 +805,20 @@
       <c r="L6" t="b">
         <v>0</v>
       </c>
-      <c r="M6" t="n">
-        <v>700</v>
+      <c r="M6" t="b">
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>3</v>
+        <v>550</v>
       </c>
       <c r="O6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Gouiri</t>
+          <t>Sørloth</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -831,7 +831,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -839,26 +839,26 @@
           <t>ST</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
+      <c r="F7" t="n">
+        <v>1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Stade Rennais FC</t>
-        </is>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
+          <t>LALIGA EA SPORTS</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Villarreal CF</t>
+        </is>
       </c>
       <c r="J7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="b">
         <v>0</v>
@@ -866,24 +866,24 @@
       <c r="L7" t="b">
         <v>0</v>
       </c>
-      <c r="M7" t="n">
-        <v>700</v>
+      <c r="M7" t="b">
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>400</v>
       </c>
       <c r="O7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Fofana</t>
+          <t>Reguilón</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -892,34 +892,34 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CB</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>Premier League</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Chelsea</t>
-        </is>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Manchester Utd</t>
+        </is>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
@@ -927,24 +927,24 @@
       <c r="L8" t="b">
         <v>0</v>
       </c>
-      <c r="M8" t="n">
-        <v>700</v>
+      <c r="M8" t="b">
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>2</v>
+        <v>450</v>
       </c>
       <c r="O8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Golovin</t>
+          <t>Luis Milla</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -953,34 +953,34 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LM</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
+          <t>CDM</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>AS Monaco</t>
-        </is>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
+          <t>LALIGA EA SPORTS</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Getafe CF</t>
+        </is>
       </c>
       <c r="J9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="b">
         <v>0</v>
@@ -988,24 +988,24 @@
       <c r="L9" t="b">
         <v>0</v>
       </c>
-      <c r="M9" t="n">
-        <v>700</v>
+      <c r="M9" t="b">
+        <v>0</v>
       </c>
       <c r="N9" t="n">
+        <v>400</v>
+      </c>
+      <c r="O9" t="n">
         <v>2</v>
-      </c>
-      <c r="O9" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ito</t>
+          <t>Chalobah</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1014,34 +1014,34 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>RW</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Japan</t>
-        </is>
+          <t>RB</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Stade de Reims</t>
-        </is>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="b">
         <v>0</v>
@@ -1049,20 +1049,20 @@
       <c r="L10" t="b">
         <v>0</v>
       </c>
-      <c r="M10" t="n">
-        <v>700</v>
+      <c r="M10" t="b">
+        <v>0</v>
       </c>
       <c r="N10" t="n">
+        <v>450</v>
+      </c>
+      <c r="O10" t="n">
         <v>2</v>
-      </c>
-      <c r="O10" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Rosier</t>
+          <t>Ferri</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1075,34 +1075,34 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RB</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
+          <t>CDM</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>France</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Süper Lig</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Beşiktaş</t>
-        </is>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
+          <t>Ligue 1 Uber Eats</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
       </c>
       <c r="J11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="b">
         <v>0</v>
@@ -1110,24 +1110,24 @@
       <c r="L11" t="b">
         <v>0</v>
       </c>
-      <c r="M11" t="n">
-        <v>700</v>
+      <c r="M11" t="b">
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Stach</t>
+          <t>Lascelles</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1136,34 +1136,34 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CM</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1. FSV Mainz 05</t>
-        </is>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Newcastle Utd</t>
+        </is>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
@@ -1171,14 +1171,14 @@
       <c r="L12" t="b">
         <v>0</v>
       </c>
-      <c r="M12" t="n">
-        <v>700</v>
+      <c r="M12" t="b">
+        <v>0</v>
       </c>
       <c r="N12" t="n">
+        <v>400</v>
+      </c>
+      <c r="O12" t="n">
         <v>2</v>
-      </c>
-      <c r="O12" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve comments and add code for fixing players
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -513,11 +513,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Shaw</t>
+          <t>Bixby</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -531,7 +531,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -539,17 +539,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>NWSL</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Portland Thorns</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="O2" t="n">
         <v>3</v>
@@ -696,7 +696,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Savanier</t>
+          <t>Mewis</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -722,17 +722,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>NWSL</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>KC Current</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -751,13 +751,13 @@
         <v>700</v>
       </c>
       <c r="O5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mandanda</t>
+          <t>Coffey</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -770,12 +770,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -783,17 +783,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>NWSL</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Stade Rennais FC</t>
+          <t>Portland Thorns</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -809,10 +809,10 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="O6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -879,7 +879,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Reguilón</t>
+          <t>Webster</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -897,7 +897,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -915,7 +915,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -931,10 +931,10 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="O8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -995,7 +995,7 @@
         <v>400</v>
       </c>
       <c r="O9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1062,7 +1062,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ferri</t>
+          <t>Diego Rico</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1088,17 +1088,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>Getafe CF</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="O11" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
Add additional objective types
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -513,11 +513,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bixby</t>
+          <t>Shaw</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -531,7 +531,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -539,17 +539,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NWSL</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Portland Thorns</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="O2" t="n">
         <v>3</v>
@@ -574,11 +574,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Gerard Moreno</t>
+          <t>Alba Redondo</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -605,12 +605,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Liga F</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Villarreal CF</t>
+          <t>Levante UD</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="O3" t="n">
         <v>3</v>
@@ -696,11 +696,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mewis</t>
+          <t>Jensen</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -714,7 +714,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -722,17 +722,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>NWSL</t>
+          <t>Liga F</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>KC Current</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -751,17 +751,17 @@
         <v>700</v>
       </c>
       <c r="O5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Coffey</t>
+          <t>Savanier</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -775,7 +775,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>CAM</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -783,17 +783,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>NWSL</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Portland Thorns</t>
+          <t>Montpellier</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -818,7 +818,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sørloth</t>
+          <t>Mandanda</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -836,7 +836,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -844,17 +844,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Villarreal CF</t>
+          <t>Stade Rennais FC</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="O7" t="n">
         <v>2</v>
@@ -879,7 +879,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Webster</t>
+          <t>Reguilón</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -897,7 +897,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -915,7 +915,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Brighton</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -931,20 +931,20 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="O8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Luis Milla</t>
+          <t>Chalobah</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -958,7 +958,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -966,17 +966,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Getafe CF</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -992,16 +992,16 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="O9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chalobah</t>
+          <t>Ferri</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>RB</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1027,17 +1027,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Montpellier</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1053,20 +1053,20 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="O10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Diego Rico</t>
+          <t>Anna Torrodà</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1093,12 +1093,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Liga F</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Getafe CF</t>
+          <t>Levante UD</t>
         </is>
       </c>
       <c r="J11" t="b">

</xml_diff>

<commit_message>
To be `Rare` or Not to be `Rare`
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,11 @@
           <t>Chemistry</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Org_Row_ID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -570,15 +575,18 @@
       <c r="O2" t="n">
         <v>3</v>
       </c>
+      <c r="P2" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alba Redondo</t>
+          <t>Botman</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -592,7 +600,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -600,17 +608,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Liga F</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Levante UD</t>
+          <t>Newcastle Utd</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -626,20 +634,23 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="O3" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>González</t>
+          <t>Giroud</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -653,15 +664,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>LW</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -671,7 +682,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Fiorentina</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -687,20 +698,23 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="P4" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jensen</t>
+          <t>Edwards</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -709,7 +723,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -722,17 +736,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Liga F</t>
+          <t>Liga Portugal</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Sporting CP</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -748,10 +762,13 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="O5" t="n">
         <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -814,6 +831,9 @@
       <c r="O6" t="n">
         <v>3</v>
       </c>
+      <c r="P6" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -875,11 +895,14 @@
       <c r="O7" t="n">
         <v>2</v>
       </c>
+      <c r="P7" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Reguilón</t>
+          <t>Malacia</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -892,7 +915,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -905,7 +928,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -931,16 +954,19 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>450</v>
+        <v>700</v>
       </c>
       <c r="O8" t="n">
         <v>3</v>
+      </c>
+      <c r="P8" t="n">
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chalobah</t>
+          <t>Loftus-Cheek</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -958,7 +984,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RB</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -971,12 +997,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Serie A TIM</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -992,20 +1018,23 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="O9" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="P9" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ferri</t>
+          <t>Walace</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1027,17 +1056,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Serie A TIM</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>Udinese</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1053,20 +1082,23 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="O10" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="P10" t="n">
+        <v>148</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Anna Torrodà</t>
+          <t>Sacko</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1075,12 +1107,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1088,17 +1120,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Mali</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Liga F</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Levante UD</t>
+          <t>Montpellier</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1114,16 +1146,19 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>400</v>
+        <v>650</v>
       </c>
       <c r="O11" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="P11" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lascelles</t>
+          <t>Maurício</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1141,7 +1176,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CAM</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1149,17 +1184,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Liga Portugal</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Newcastle Utd</t>
+          <t>Portimonense SC</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1178,7 +1213,10 @@
         <v>400</v>
       </c>
       <c r="O12" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P12" t="n">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Rarity` col is now more detailed. Relevant changes made like `Radioactive` chem.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -518,11 +518,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Shaw</t>
+          <t>Zelem</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -536,7 +536,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -549,7 +549,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Barclays WSL</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -570,23 +570,23 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="O2" t="n">
         <v>3</v>
       </c>
       <c r="P2" t="n">
-        <v>26</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Botman</t>
+          <t>van de Donk</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CAM</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -613,12 +613,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>D1 Arkema</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Newcastle Utd</t>
+          <t>OL</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -634,19 +634,19 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="O3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P3" t="n">
-        <v>33</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Giroud</t>
+          <t>Lopes</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -659,12 +659,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -672,17 +672,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Serie A TIM</t>
+          <t>Ligue 1 Uber Eats</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>OL</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -698,23 +698,23 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="O4" t="n">
         <v>3</v>
       </c>
       <c r="P4" t="n">
-        <v>38</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Edwards</t>
+          <t>Pacheco</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -723,12 +723,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -741,12 +741,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Liga Portugal</t>
+          <t>Barclays WSL</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Sporting CP</t>
+          <t>Aston Villa</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -762,23 +762,23 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" t="n">
-        <v>56</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Savanier</t>
+          <t>Le Tissier</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -800,17 +800,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>England</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Barclays WSL</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -832,17 +832,17 @@
         <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>60</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mandanda</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -851,12 +851,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -874,7 +874,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Stade Rennais FC</t>
+          <t>Paris SG</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -890,23 +890,23 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="O7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P7" t="n">
-        <v>70</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Malacia</t>
+          <t>Groenen</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -920,7 +920,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -933,12 +933,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>D1 Arkema</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Paris SG</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -960,17 +960,17 @@
         <v>3</v>
       </c>
       <c r="P8" t="n">
-        <v>104</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Loftus-Cheek</t>
+          <t>Cissoko</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -992,17 +992,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Serie A TIM</t>
+          <t>Barclays WSL</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>West Ham</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -1018,23 +1018,23 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="O9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P9" t="n">
-        <v>115</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Walace</t>
+          <t>Cambot</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1056,17 +1056,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Serie A TIM</t>
+          <t>D1 Arkema</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Udinese</t>
+          <t>En Avant Guingamp</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1082,23 +1082,23 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="O10" t="n">
         <v>2</v>
       </c>
       <c r="P10" t="n">
-        <v>148</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sacko</t>
+          <t>Guilbert</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Mali</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>Strasbourg</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1146,27 +1146,27 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="O11" t="n">
         <v>2</v>
       </c>
       <c r="P11" t="n">
-        <v>155</v>
+        <v>635</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Maurício</t>
+          <t>Jurić</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>Bronze</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1176,25 +1176,25 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Bosnia Herzegovina</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Liga Portugal</t>
+          <t>PKO BP Ekstraklasa</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Portimonense SC</t>
+          <t>ŁKS Łódź</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1210,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>158</v>
+        <v>833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add chemistry rules for `Fire` and `Ice` cards.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -518,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Zelem</t>
+          <t>Mario Hermoso</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -544,17 +544,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Barclays WSL</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Atlético de Madrid</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -573,16 +573,16 @@
         <v>750</v>
       </c>
       <c r="O2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P2" t="n">
-        <v>147</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>van de Donk</t>
+          <t>David García</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -595,12 +595,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -608,17 +608,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>D1 Arkema</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>OL</t>
+          <t>CA Osasuna</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -634,23 +634,23 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="O3" t="n">
         <v>3</v>
       </c>
       <c r="P3" t="n">
-        <v>169</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lopes</t>
+          <t>Mertens</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -664,7 +664,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -672,17 +672,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Trendyol Süper Lig</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>OL</t>
+          <t>Galatasaray</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -698,19 +698,19 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="O4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P4" t="n">
-        <v>171</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pacheco</t>
+          <t>Fred</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -728,7 +728,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -736,17 +736,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Barclays WSL</t>
+          <t>Trendyol Süper Lig</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>Fenerbahçe</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -765,16 +765,16 @@
         <v>700</v>
       </c>
       <c r="O5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P5" t="n">
-        <v>205</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Le Tissier</t>
+          <t>Lo Celso</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -792,7 +792,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -800,17 +800,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Barclays WSL</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Spurs</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -829,16 +829,16 @@
         <v>700</v>
       </c>
       <c r="O6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6" t="n">
-        <v>226</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Kamara</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -856,7 +856,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>CDM</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -864,17 +864,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Paris SG</t>
+          <t>Aston Villa</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -896,17 +896,17 @@
         <v>3</v>
       </c>
       <c r="P7" t="n">
-        <v>296</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Groenen</t>
+          <t>Lamela</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -920,7 +920,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>CAM</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -928,17 +928,17 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>D1 Arkema</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Paris SG</t>
+          <t>Sevilla FC</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -957,16 +957,16 @@
         <v>700</v>
       </c>
       <c r="O8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P8" t="n">
-        <v>347</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cissoko</t>
+          <t>Digne</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -997,12 +997,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Barclays WSL</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Aston Villa</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -1018,23 +1018,23 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="O9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P9" t="n">
-        <v>372</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cambot</t>
+          <t>Nacho Vidal</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1056,17 +1056,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>D1 Arkema</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>En Avant Guingamp</t>
+          <t>CA Osasuna</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1082,23 +1082,23 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="O10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P10" t="n">
-        <v>497</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Guilbert</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RB</t>
+          <t>CAM</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1120,17 +1120,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Ligue 1 Uber Eats</t>
+          <t>Trendyol Süper Lig</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Strasbourg</t>
+          <t>Fenerbahçe</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1146,23 +1146,23 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>500</v>
+        <v>650</v>
       </c>
       <c r="O11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P11" t="n">
-        <v>635</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jurić</t>
+          <t>Barrea</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1184,17 +1184,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Bosnia Herzegovina</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>PKO BP Ekstraklasa</t>
+          <t>LPF</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ŁKS Łódź</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>833</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add an example SBC
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -518,11 +518,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mario Hermoso</t>
+          <t>Aké</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -536,7 +536,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -544,17 +544,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Atlético de Madrid</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -570,23 +570,23 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="O2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P2" t="n">
-        <v>48</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>David García</t>
+          <t>Danjuma</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -595,12 +595,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>Rare</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>LM</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -608,17 +608,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>CA Osasuna</t>
+          <t>Everton</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -640,17 +640,17 @@
         <v>3</v>
       </c>
       <c r="P3" t="n">
-        <v>61</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mertens</t>
+          <t>Dalot Teixeira</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -664,7 +664,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -672,17 +672,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Trendyol Süper Lig</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Galatasaray</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -701,20 +701,20 @@
         <v>700</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P4" t="n">
-        <v>108</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fred</t>
+          <t>García Córdoba</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -736,17 +736,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Trendyol Süper Lig</t>
+          <t>Barclays WSL</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Fenerbahçe</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -762,23 +762,23 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="O5" t="n">
         <v>3</v>
       </c>
       <c r="P5" t="n">
-        <v>111</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lo Celso</t>
+          <t>Elustondo</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -787,12 +787,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -800,17 +800,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Spurs</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -826,19 +826,19 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>700</v>
+        <v>550</v>
       </c>
       <c r="O6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>115</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kamara</t>
+          <t>Martial</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -856,7 +856,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CDM</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -874,7 +874,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -896,17 +896,17 @@
         <v>3</v>
       </c>
       <c r="P7" t="n">
-        <v>118</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lamela</t>
+          <t>Catena Marugán</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -915,12 +915,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rare</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -928,7 +928,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Sevilla FC</t>
+          <t>CA Osasuna</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -954,19 +954,19 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="O8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P8" t="n">
-        <v>125</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Digne</t>
+          <t>Pinillos Moreno</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -992,17 +992,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Liga F</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>Madrid CFF</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -1018,23 +1018,23 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="O9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P9" t="n">
-        <v>147</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nacho Vidal</t>
+          <t>McTominay</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>RB</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1056,17 +1056,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Scotland</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LALIGA EA SPORTS</t>
+          <t>Premier League</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>CA Osasuna</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1082,23 +1082,23 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="O10" t="n">
         <v>3</v>
       </c>
       <c r="P10" t="n">
-        <v>195</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Herrera Pirón</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CAM</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1120,17 +1120,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Trendyol Süper Lig</t>
+          <t>LALIGA EA SPORTS</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Fenerbahçe</t>
+          <t>CA Osasuna</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1146,27 +1146,27 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="O11" t="n">
         <v>3</v>
       </c>
       <c r="P11" t="n">
-        <v>223</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Barrea</t>
+          <t>Maitane</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bronze</t>
+          <t>Gold</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1176,25 +1176,25 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>LPF</t>
+          <t>NWSL</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>NJ/NY Gotham</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1210,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P12" t="n">
-        <v>239</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>